<commit_message>
Adding new version of qNTA_Surrogate_Detection_Statistics_File_WW2DW.xlsx
New file has single sheet named 'Surrogate Detection Statistics' as opposed to 'Sheet 1'
</commit_message>
<xml_diff>
--- a/data/qNTA_Surrogate_Detection_Statistics_File_WW2DW.xlsx
+++ b/data/qNTA_Surrogate_Detection_Statistics_File_WW2DW.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/carr_erik_epa_gov/Documents/Profile/projects/NTAWebApp/jobs/qNTA/interactive_strip_plots-2025_02_13/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/ferland_troy_epa_gov/Documents/Profile/Documents/WebApp Admin/Proposed Additions/qNTA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="8_{525C2709-35CF-46C1-ABAA-ABE2F5D1A4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7503635-98C5-40A2-9C4D-C54655A9FE60}"/>
+  <xr:revisionPtr revIDLastSave="145" documentId="8_{525C2709-35CF-46C1-ABAA-ABE2F5D1A4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{536C1827-A74D-43ED-902B-04B489754300}"/>
   <bookViews>
-    <workbookView xWindow="72" yWindow="3108" windowWidth="17280" windowHeight="8880" xr2:uid="{A3A4EB2A-C2F9-464F-802B-39AF53C55C65}"/>
+    <workbookView xWindow="2952" yWindow="336" windowWidth="19218" windowHeight="13344" xr2:uid="{A3A4EB2A-C2F9-464F-802B-39AF53C55C65}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Surrogate Detection Statistics" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1132,76 +1132,74 @@
   <dimension ref="A1:CC74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AI1" sqref="AI1"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.734375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" style="2" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="8.77734375" style="2" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" style="2" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="31.77734375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="22.33203125" style="2" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="23" style="2" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="11.88671875" style="2" hidden="1" customWidth="1"/>
-    <col min="14" max="15" width="8.77734375" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="9.109375" style="2" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="16.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="15.88671875" style="2" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="17.77734375" style="2" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="31.44140625" style="2" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="19.44140625" style="2" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="23.77734375" style="2" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="20.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="24" max="30" width="9.77734375" style="2" hidden="1" customWidth="1"/>
-    <col min="31" max="35" width="10.77734375" style="2" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="9.77734375" style="2" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="8.77734375" style="2" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="9.77734375" style="2" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="8.21875" style="2" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="9.77734375" style="2" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="12.33203125" style="2" hidden="1" customWidth="1"/>
-    <col min="42" max="44" width="13.44140625" style="2" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="14.44140625" style="2" hidden="1" customWidth="1"/>
-    <col min="46" max="46" width="8.88671875" style="2" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="10.77734375" style="2" hidden="1" customWidth="1"/>
-    <col min="48" max="50" width="11.77734375" style="2" hidden="1" customWidth="1"/>
-    <col min="51" max="51" width="12.77734375" style="2" hidden="1" customWidth="1"/>
-    <col min="52" max="52" width="9.77734375" style="2" hidden="1" customWidth="1"/>
-    <col min="53" max="55" width="10.77734375" style="2" hidden="1" customWidth="1"/>
-    <col min="56" max="56" width="11.77734375" style="2" hidden="1" customWidth="1"/>
-    <col min="57" max="57" width="21.5546875" style="2" hidden="1" customWidth="1"/>
-    <col min="58" max="60" width="22.5546875" style="2" hidden="1" customWidth="1"/>
-    <col min="61" max="61" width="23.5546875" style="2" hidden="1" customWidth="1"/>
-    <col min="62" max="62" width="25.88671875" style="2" hidden="1" customWidth="1"/>
-    <col min="63" max="65" width="26.88671875" style="2" hidden="1" customWidth="1"/>
-    <col min="66" max="66" width="27.88671875" style="2" hidden="1" customWidth="1"/>
-    <col min="67" max="67" width="20.77734375" style="2" hidden="1" customWidth="1"/>
-    <col min="68" max="69" width="21.77734375" style="2" hidden="1" customWidth="1"/>
-    <col min="70" max="70" width="33.109375" style="2" customWidth="1"/>
-    <col min="71" max="71" width="10.6640625" style="2" customWidth="1"/>
-    <col min="72" max="72" width="17" style="2" customWidth="1"/>
-    <col min="73" max="73" width="13.5546875" style="2" customWidth="1"/>
-    <col min="74" max="74" width="19.5546875" style="2" customWidth="1"/>
-    <col min="75" max="75" width="24.5546875" style="2" customWidth="1"/>
-    <col min="76" max="76" width="23.21875" style="2" customWidth="1"/>
-    <col min="77" max="77" width="9.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="10.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="11.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="10.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="11.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="82" max="16384" width="8.77734375" style="2"/>
+    <col min="1" max="1" width="9.5234375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.5234375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.7890625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.62890625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.89453125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.62890625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.7890625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="13.734375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.62890625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.734375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="22.3671875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="23" style="2" customWidth="1"/>
+    <col min="13" max="13" width="11.89453125" style="2" customWidth="1"/>
+    <col min="14" max="15" width="8.7890625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="9.1015625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="16.62890625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="15.89453125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="17.734375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="31.47265625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="19.47265625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="23.7890625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="20.62890625" style="2" customWidth="1"/>
+    <col min="24" max="30" width="9.7890625" style="2" customWidth="1"/>
+    <col min="31" max="35" width="10.7890625" style="2" customWidth="1"/>
+    <col min="36" max="36" width="9.7890625" style="2" customWidth="1"/>
+    <col min="37" max="37" width="8.7890625" style="2" customWidth="1"/>
+    <col min="38" max="38" width="9.7890625" style="2" customWidth="1"/>
+    <col min="39" max="39" width="8.26171875" style="2" customWidth="1"/>
+    <col min="40" max="40" width="9.7890625" style="2" customWidth="1"/>
+    <col min="41" max="41" width="12.3671875" style="2" customWidth="1"/>
+    <col min="42" max="44" width="13.47265625" style="2" customWidth="1"/>
+    <col min="45" max="45" width="14.47265625" style="2" customWidth="1"/>
+    <col min="46" max="46" width="8.89453125" style="2" customWidth="1"/>
+    <col min="47" max="47" width="10.734375" style="2" customWidth="1"/>
+    <col min="48" max="50" width="11.734375" style="2" customWidth="1"/>
+    <col min="51" max="51" width="12.734375" style="2" customWidth="1"/>
+    <col min="52" max="52" width="9.7890625" style="2" customWidth="1"/>
+    <col min="53" max="55" width="10.7890625" style="2" customWidth="1"/>
+    <col min="56" max="56" width="11.7890625" style="2" customWidth="1"/>
+    <col min="57" max="57" width="21.5234375" style="2" customWidth="1"/>
+    <col min="58" max="60" width="22.5234375" style="2" customWidth="1"/>
+    <col min="61" max="61" width="23.5234375" style="2" customWidth="1"/>
+    <col min="62" max="62" width="25.89453125" style="2" customWidth="1"/>
+    <col min="63" max="65" width="26.89453125" style="2" customWidth="1"/>
+    <col min="66" max="66" width="27.89453125" style="2" customWidth="1"/>
+    <col min="67" max="67" width="20.734375" style="2" customWidth="1"/>
+    <col min="68" max="69" width="21.7890625" style="2" customWidth="1"/>
+    <col min="70" max="70" width="22.62890625" style="2" customWidth="1"/>
+    <col min="71" max="71" width="22.7890625" style="2" customWidth="1"/>
+    <col min="72" max="72" width="11.62890625" style="2" customWidth="1"/>
+    <col min="73" max="75" width="12.62890625" style="2" customWidth="1"/>
+    <col min="76" max="76" width="13.734375" style="2" customWidth="1"/>
+    <col min="77" max="77" width="9.7890625" style="6" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="10.5234375" style="6" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="11.7890625" style="6" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="10.7890625" style="6" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="11.5234375" style="6" bestFit="1" customWidth="1"/>
+    <col min="82" max="16384" width="8.734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1446,7 +1444,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2">
         <v>2565</v>
       </c>
@@ -1674,7 +1672,7 @@
         <v>188.1165</v>
       </c>
     </row>
-    <row r="3" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2">
         <v>401</v>
       </c>
@@ -1899,7 +1897,7 @@
         <v>21.24663</v>
       </c>
     </row>
-    <row r="4" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2">
         <v>1687</v>
       </c>
@@ -2127,7 +2125,7 @@
         <v>56.345120000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2">
         <v>2791</v>
       </c>
@@ -2355,7 +2353,7 @@
         <v>83.101119999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2">
         <v>2325</v>
       </c>
@@ -2580,7 +2578,7 @@
         <v>333.46800000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2">
         <v>3815</v>
       </c>
@@ -2770,7 +2768,7 @@
         <v>5.1562719999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2">
         <v>247</v>
       </c>
@@ -2995,7 +2993,7 @@
         <v>26.266582</v>
       </c>
     </row>
-    <row r="9" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2">
         <v>2136</v>
       </c>
@@ -3220,7 +3218,7 @@
         <v>109.77916</v>
       </c>
     </row>
-    <row r="10" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2">
         <v>4522</v>
       </c>
@@ -3411,7 +3409,7 @@
         <v>6.0210020000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2">
         <v>2788</v>
       </c>
@@ -3636,7 +3634,7 @@
         <v>362.89825000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2">
         <v>3724</v>
       </c>
@@ -3823,7 +3821,7 @@
         <v>9.1666640000000008</v>
       </c>
     </row>
-    <row r="13" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2">
         <v>997</v>
       </c>
@@ -4029,7 +4027,7 @@
         <v>30.430443</v>
       </c>
     </row>
-    <row r="14" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2">
         <v>1621</v>
       </c>
@@ -4257,7 +4255,7 @@
         <v>102.99894500000001</v>
       </c>
     </row>
-    <row r="15" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2">
         <v>1900</v>
       </c>
@@ -4482,7 +4480,7 @@
         <v>53.864305000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2">
         <v>1535</v>
       </c>
@@ -4707,7 +4705,7 @@
         <v>129.75742</v>
       </c>
     </row>
-    <row r="17" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2">
         <v>2722</v>
       </c>
@@ -4932,7 +4930,7 @@
         <v>296.089</v>
       </c>
     </row>
-    <row r="18" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2">
         <v>2532</v>
       </c>
@@ -5116,7 +5114,7 @@
         <v>3.2594546000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2">
         <v>3863</v>
       </c>
@@ -5341,7 +5339,7 @@
         <v>202.42964000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2">
         <v>3600</v>
       </c>
@@ -5566,7 +5564,7 @@
         <v>161.13446999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2">
         <v>3190</v>
       </c>
@@ -5791,7 +5789,7 @@
         <v>295.07079999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2">
         <v>4297</v>
       </c>
@@ -6000,7 +5998,7 @@
         <v>48.310195</v>
       </c>
     </row>
-    <row r="23" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2">
         <v>4318</v>
       </c>
@@ -6209,7 +6207,7 @@
         <v>6.0390930000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2">
         <v>669</v>
       </c>
@@ -6434,7 +6432,7 @@
         <v>93.761690000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2">
         <v>3528</v>
       </c>
@@ -6662,7 +6660,7 @@
         <v>171.88800000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2">
         <v>2660</v>
       </c>
@@ -6868,7 +6866,7 @@
         <v>65.902240000000006</v>
       </c>
     </row>
-    <row r="27" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2">
         <v>3469</v>
       </c>
@@ -7074,7 +7072,7 @@
         <v>29.874020000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2">
         <v>983</v>
       </c>
@@ -7280,7 +7278,7 @@
         <v>99.623100000000008</v>
       </c>
     </row>
-    <row r="29" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2">
         <v>200</v>
       </c>
@@ -7508,7 +7506,7 @@
         <v>19.737432000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2">
         <v>373</v>
       </c>
@@ -7733,7 +7731,7 @@
         <v>103.01491</v>
       </c>
     </row>
-    <row r="31" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2">
         <v>3580</v>
       </c>
@@ -7942,7 +7940,7 @@
         <v>14.081781000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2">
         <v>2155</v>
       </c>
@@ -8167,7 +8165,7 @@
         <v>188.70157999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2">
         <v>3778</v>
       </c>
@@ -8395,7 +8393,7 @@
         <v>144.08828</v>
       </c>
     </row>
-    <row r="34" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2">
         <v>2653</v>
       </c>
@@ -8601,7 +8599,7 @@
         <v>59.099694999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2">
         <v>2599</v>
       </c>
@@ -8807,7 +8805,7 @@
         <v>19.715828000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2">
         <v>4044</v>
       </c>
@@ -9035,7 +9033,7 @@
         <v>222.00670000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2">
         <v>2907</v>
       </c>
@@ -9263,7 +9261,7 @@
         <v>69.57687</v>
       </c>
     </row>
-    <row r="38" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2">
         <v>3097</v>
       </c>
@@ -9469,7 +9467,7 @@
         <v>214.02462</v>
       </c>
     </row>
-    <row r="39" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2">
         <v>3447</v>
       </c>
@@ -9678,7 +9676,7 @@
         <v>14.914346999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="2">
         <v>3420</v>
       </c>
@@ -9884,7 +9882,7 @@
         <v>28.918071999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2">
         <v>2901</v>
       </c>
@@ -10090,7 +10088,7 @@
         <v>49.351027000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2">
         <v>2448</v>
       </c>
@@ -10315,7 +10313,7 @@
         <v>213.62764000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="2">
         <v>2035</v>
       </c>
@@ -10543,7 +10541,7 @@
         <v>256.49235999999996</v>
       </c>
     </row>
-    <row r="44" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2">
         <v>3233</v>
       </c>
@@ -10749,7 +10747,7 @@
         <v>27.077642999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2">
         <v>2888</v>
       </c>
@@ -10974,7 +10972,7 @@
         <v>47.849510000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="2">
         <v>2755</v>
       </c>
@@ -11180,7 +11178,7 @@
         <v>36.68477</v>
       </c>
     </row>
-    <row r="47" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2">
         <v>3898</v>
       </c>
@@ -11351,7 +11349,7 @@
         <v>1.2304774000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="2">
         <v>1916</v>
       </c>
@@ -11560,7 +11558,7 @@
         <v>51.310883000000004</v>
       </c>
     </row>
-    <row r="49" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="2">
         <v>793</v>
       </c>
@@ -11769,7 +11767,7 @@
         <v>28.280389</v>
       </c>
     </row>
-    <row r="50" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="2">
         <v>2092</v>
       </c>
@@ -11994,7 +11992,7 @@
         <v>101.86691</v>
       </c>
     </row>
-    <row r="51" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="2">
         <v>1918</v>
       </c>
@@ -12219,7 +12217,7 @@
         <v>97.34653999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="2">
         <v>2517</v>
       </c>
@@ -12444,7 +12442,7 @@
         <v>141.97696999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="2">
         <v>4004</v>
       </c>
@@ -12672,7 +12670,7 @@
         <v>16.406059000000003</v>
       </c>
     </row>
-    <row r="54" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="2">
         <v>4119</v>
       </c>
@@ -12897,7 +12895,7 @@
         <v>224.73694</v>
       </c>
     </row>
-    <row r="55" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="2">
         <v>2794</v>
       </c>
@@ -13122,7 +13120,7 @@
         <v>76.028700000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="2">
         <v>5194</v>
       </c>
@@ -13294,7 +13292,7 @@
         <v>2.4556390000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="2">
         <v>5097</v>
       </c>
@@ -13500,7 +13498,7 @@
         <v>14.401584000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="2">
         <v>5075</v>
       </c>
@@ -13703,7 +13701,7 @@
         <v>1.9939435000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="2">
         <v>5219</v>
       </c>
@@ -13909,7 +13907,7 @@
         <v>6.6281189999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="2">
         <v>5734</v>
       </c>
@@ -14115,7 +14113,7 @@
         <v>4.2109633999999998</v>
       </c>
     </row>
-    <row r="61" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="2">
         <v>5879</v>
       </c>
@@ -14249,7 +14247,7 @@
         <v>2.2660704000000003</v>
       </c>
     </row>
-    <row r="62" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="2">
         <v>5833</v>
       </c>
@@ -14386,7 +14384,7 @@
         <v>0.84997319999999998</v>
       </c>
     </row>
-    <row r="63" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="2">
         <v>5563</v>
       </c>
@@ -14573,7 +14571,7 @@
         <v>11.027376</v>
       </c>
     </row>
-    <row r="64" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="2">
         <v>5120</v>
       </c>
@@ -14779,7 +14777,7 @@
         <v>4.005547</v>
       </c>
     </row>
-    <row r="65" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="2">
         <v>5246</v>
       </c>
@@ -14966,7 +14964,7 @@
         <v>12.783560999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="2">
         <v>5787</v>
       </c>
@@ -15191,7 +15189,7 @@
         <v>17.405006</v>
       </c>
     </row>
-    <row r="67" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="2">
         <v>5832</v>
       </c>
@@ -15397,7 +15395,7 @@
         <v>9.5516200000000016</v>
       </c>
     </row>
-    <row r="68" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="2">
         <v>5410</v>
       </c>
@@ -15622,7 +15620,7 @@
         <v>6.6724287000000002</v>
       </c>
     </row>
-    <row r="69" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="2">
         <v>5167</v>
       </c>
@@ -15828,7 +15826,7 @@
         <v>4.1347589999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="2">
         <v>5636</v>
       </c>
@@ -16000,7 +15998,7 @@
         <v>1.8149884999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="2">
         <v>5493</v>
       </c>
@@ -16206,7 +16204,7 @@
         <v>3.6589504000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="2">
         <v>5708</v>
       </c>
@@ -16396,7 +16394,7 @@
         <v>5.8847934999999998</v>
       </c>
     </row>
-    <row r="73" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="2">
         <v>5136</v>
       </c>
@@ -16602,7 +16600,7 @@
         <v>14.921139999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:81" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="2">
         <v>5464</v>
       </c>

</xml_diff>